<commit_message>
Updated problem 2 and 3 to completion. Problem 1 also updated.
</commit_message>
<xml_diff>
--- a/Asssignment4_Data.xlsx
+++ b/Asssignment4_Data.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saakur/Desktop/OSU_Teaching/Machine Learning/Assignments/Solutions/Assn1/Assn3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92d6ee6f6bb378a7/MachineLearning/hw/4/ML_Assignment4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FD104879-78B0-4345-A915-579F52A407CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="13_ncr:40009_{FD104879-78B0-4345-A915-579F52A407CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8768898-0366-4004-B971-DEC0A6CEE95F}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" activeTab="1"/>
+    <workbookView xWindow="-8280" yWindow="675" windowWidth="36255" windowHeight="14910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Train" sheetId="1" r:id="rId1"/>
     <sheet name="Test" sheetId="2" r:id="rId2"/>
+    <sheet name="House" sheetId="6" r:id="rId3"/>
+    <sheet name="Condo" sheetId="5" r:id="rId4"/>
+    <sheet name="Apartment" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="15">
   <si>
     <t>House ID</t>
   </si>
@@ -71,11 +74,17 @@
   <si>
     <t>Condo</t>
   </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -212,7 +221,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,8 +401,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -508,6 +523,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -553,8 +577,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -611,6 +638,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>257733</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76294</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{750F9B58-7DDD-404D-7605-2C9356161129}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="2400300"/>
+          <a:ext cx="4001058" cy="676369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -909,16 +985,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:J29"/>
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -950,7 +1026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -982,7 +1058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1014,7 +1090,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1046,7 +1122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1078,7 +1154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1110,7 +1186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1142,7 +1218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1174,7 +1250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1206,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1238,7 +1314,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1270,7 +1346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1302,7 +1378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1334,7 +1410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1366,7 +1442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1398,7 +1474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1430,7 +1506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1462,7 +1538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1494,7 +1570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1526,7 +1602,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1558,7 +1634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1596,16 +1672,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>24</v>
       </c>
@@ -1669,7 +1745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25</v>
       </c>
@@ -1701,7 +1777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>26</v>
       </c>
@@ -1733,7 +1809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>27</v>
       </c>
@@ -1765,7 +1841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>28</v>
       </c>
@@ -1800,4 +1876,1012 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599214AB-C5CE-45DC-BEFE-CF5BF6022E37}">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.125" customWidth="1"/>
+    <col min="10" max="11" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>5.0208000000000004</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3.5310000000000001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2">
+        <v>62</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>5.6039000000000003</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9.52</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>5.8281999999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.4349999999999996</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2">
+        <v>32</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>5.3003</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4.9882999999999997</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.552</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>6.2712000000000003</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5.52</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>30</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>5.6039000000000003</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>9.52</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>32</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>6.6969000000000003</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6.9020000000000001</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.488</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>7</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>22</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <f>_xlfn.VAR.S(B2:B8)</f>
+        <v>0.32503826285714288</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:I9" si="0">_xlfn.VAR.S(C2:C8)</f>
+        <v>3.5714285714285587E-2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>5.0578805366666684</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>4.5336571428571837E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.70238095238095222</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047211</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>161.90476190476178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(B2:B8)</f>
+        <v>5.7607428571428576</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:I10" si="1">AVERAGE(C2:C8)</f>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>6.6308999999999996</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>1.3917142857142857</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>6.1428571428571432</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>34.285714285714285</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>6.0930999999999997</v>
+      </c>
+      <c r="C17">
+        <v>1.5</v>
+      </c>
+      <c r="D17">
+        <v>6.7264999999999997</v>
+      </c>
+      <c r="E17">
+        <v>1.6519999999999999</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>(1/SQRT(2*PI()*B9)*EXP(-((B17-B10)^2/(2*B9))))</f>
+        <v>0.59040132685648516</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:I18" si="2">(1/SQRT(2*PI()*C9)*EXP(-((C17-C10)^2/(2*C9))))</f>
+        <v>0.16133620692951636</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>0.1772284368064895</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0.88754830870281931</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>0.47429261478135654</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>0.56586574290252301</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>0.690988298942671</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>2.3426878989545687E-2</v>
+      </c>
+      <c r="J18">
+        <f>PRODUCT(B18:I18)</f>
+        <v>6.5095275201504922E-5</v>
+      </c>
+      <c r="K18">
+        <f>0.35*J18</f>
+        <v>2.2783346320526722E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A2EFE2B-0D4D-41D3-BA6F-3E455BEF1A2B}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>4.5429000000000004</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.2749999999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.175</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
+        <v>40</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>3.891</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.4550000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>56</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>5.8979999999999997</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5.85</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2">
+        <v>51</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>16.420200000000001</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.42</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>42</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>5.9592000000000001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.6660000000000004</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.121</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2">
+        <v>32</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>7.7840999999999996</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.1020000000000003</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.3759999999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>17</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <f>_xlfn.VAR.S(B2:B7)</f>
+        <v>21.263606807999999</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:I8" si="0">_xlfn.VAR.S(C2:C7)</f>
+        <v>0.36666666666666681</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>6.4758918666666601</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.8527438666666658</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666677</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>2.5666666666666629</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666574</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>194.6666666666668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <f>AVERAGE(B2:B7)</f>
+        <v>7.4159000000000006</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:I9" si="1">AVERAGE(C2:C7)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>6.0246666666666675</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1.5533333333333335</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>6.833333333333333</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>39.666666666666664</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D8713E-5479-4993-A487-0273295AB253}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>4.9176000000000002</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3.472</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.998</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1">
+        <v>42</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>4.5572999999999997</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4.05</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.232</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>54</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>5.0597000000000003</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.4550000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.121</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>14.4598</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>12.8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>9</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>5.05</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>46</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>8.2463999999999995</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5.15</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.6639999999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2">
+        <v>50</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>9.0383999999999993</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1">
+        <v>23</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <f>_xlfn.VAR.S(B2:B8)</f>
+        <v>13.075436006190481</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:I9" si="0">_xlfn.VAR.S(C2:C8)</f>
+        <v>0.32142857142857145</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>10.61788414285715</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.49576500000000018</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.48809523809523814</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1.8095238095238055</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.95238095238095133</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>215.57142857142844</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(B2:B8)</f>
+        <v>7.3327428571428568</v>
+      </c>
+      <c r="C10">
+        <f>AVERAGE(C2:C8)</f>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="D10">
+        <f>AVERAGE(D2:D8)</f>
+        <v>6.1038571428571426</v>
+      </c>
+      <c r="E10">
+        <f>AVERAGE(E2:E8)</f>
+        <v>1.5050000000000001</v>
+      </c>
+      <c r="F10">
+        <f>AVERAGE(F2:F8)</f>
+        <v>1.2142857142857142</v>
+      </c>
+      <c r="G10">
+        <f>AVERAGE(G2:G8)</f>
+        <v>6.8571428571428568</v>
+      </c>
+      <c r="H10">
+        <f>AVERAGE(H2:H8)</f>
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="I10">
+        <f>AVERAGE(I2:I8)</f>
+        <v>38.714285714285715</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>